<commit_message>
Polished code and script fixes
</commit_message>
<xml_diff>
--- a/public/static/schedule.xlsx
+++ b/public/static/schedule.xlsx
@@ -1,78 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="198"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28515" windowHeight="13860"/>
   </bookViews>
   <sheets>
-    <sheet name="Orria1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Excerpt</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t>End date</t>
-  </si>
-  <si>
-    <t>Lecturer</t>
-  </si>
-  <si>
-    <t>Excerpt</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>lec</t>
-  </si>
-  <si>
-    <t>exc</t>
-  </si>
-  <si>
-    <t>micasa</t>
+    <t>Starts</t>
+  </si>
+  <si>
+    <t>Ends</t>
+  </si>
+  <si>
+    <t>The id</t>
+  </si>
+  <si>
+    <t>Title of the events</t>
+  </si>
+  <si>
+    <t>"YYYY-MM-DD"</t>
+  </si>
+  <si>
+    <t>"HH:MM:SS"</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Lecturer(s)</t>
+  </si>
+  <si>
+    <t>Excerpt of paper, outline, etc</t>
+  </si>
+  <si>
+    <t>More accurate is better</t>
+  </si>
+  <si>
+    <t>Lecturer list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,11 +108,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,73 +414,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="1026" width="11.5703125"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>41286</v>
-      </c>
-      <c r="E2" s="3">
-        <v>41317</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Arrunta"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Arrunta"&amp;12Orrialdea &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>